<commit_message>
Added some further notes about variant 9.
</commit_message>
<xml_diff>
--- a/Day3/assessing-variants.xlsx
+++ b/Day3/assessing-variants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Chromosome</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Nothing to suggest this isn't real, note that the allele fraction is 17% possibly reflective of the cellularity of the tumour sample and the copy number at this locus</t>
   </si>
   <si>
-    <t>Filtered by cgpCaVEManPostProcessor, DTH filter (&lt; 1/3 mutant alleles with base quality &gt;= 25), 2 variant supporting reads in normal but with very low base qualities</t>
-  </si>
-  <si>
     <t>IGV</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>Zoom out and turn on colouring of reads base insert size and orientation</t>
+  </si>
+  <si>
+    <t>Filtered by cgpCaVEManPostProcessor, SE strand bias filter and DTH filter (&lt; 1/3 mutant alleles with base quality &gt;= 25), 2 variant supporting reads in normal but with very low base qualities</t>
+  </si>
+  <si>
+    <t>Several of the variant reads are soft-clipped as evident from tooltips; zoom out and turn on display of soft-clipped bases to see lots with very low base qualities</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCellId="1" sqref="A1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45">
@@ -583,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A2&amp;":"&amp;B2, "IGV")</f>
+        <f t="shared" ref="E2:E7" si="0">HYPERLINK("http://localhost:60151/goto?locus="&amp;A2&amp;":"&amp;B2, "IGV")</f>
         <v>IGV</v>
       </c>
       <c r="F2" s="2" t="b">
@@ -593,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45">
@@ -610,17 +613,17 @@
         <v>10</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A3&amp;":"&amp;B3, "IGV")</f>
+        <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
@@ -637,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A4&amp;":"&amp;B4, "IGV")</f>
+        <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
       <c r="F4" s="2" t="b">
@@ -661,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A5&amp;":"&amp;B5, "IGV")</f>
+        <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -671,7 +674,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
@@ -688,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A6&amp;":"&amp;B6, "IGV")</f>
+        <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
       <c r="F6" s="2" t="b">
@@ -712,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A7&amp;":"&amp;B7, "IGV")</f>
+        <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
       <c r="F7" s="2" t="b">
@@ -736,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" ref="E8:E11" si="0">HYPERLINK("http://localhost:60151/goto?locus="&amp;A8&amp;":"&amp;B8, "IGV")</f>
+        <f t="shared" ref="E8:E11" si="1">HYPERLINK("http://localhost:60151/goto?locus="&amp;A8&amp;":"&amp;B8, "IGV")</f>
         <v>IGV</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -760,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>IGV</v>
       </c>
       <c r="F9" s="2" t="b">
@@ -770,10 +773,10 @@
         <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -787,14 +790,17 @@
         <v>5</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IGV</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>IGV</v>
+      </c>
+      <c r="F10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45">
@@ -811,17 +817,17 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>IGV</v>
       </c>
       <c r="F11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>